<commit_message>
Update GST column handling to flexible search in generate_master_payout.py
</commit_message>
<xml_diff>
--- a/outputs/Dosa_Coffee_Master_output_Report_Period_UNKNOWN.xlsx
+++ b/outputs/Dosa_Coffee_Master_output_Report_Period_UNKNOWN.xlsx
@@ -451,7 +451,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>(20) GST to be paid by Restaurant partner to Govt.</t>
+          <t>(19) GST paid by Zomato on behalf of restaurant - under section 9(5)</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -486,7 +486,7 @@
         <v>255.78</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>12784.6</v>
       </c>
       <c r="E2" t="n">
         <v>193974.07</v>
@@ -514,7 +514,7 @@
         <v>343.03</v>
       </c>
       <c r="D3" t="n">
-        <v>0.4</v>
+        <v>17158.95</v>
       </c>
       <c r="E3" t="n">
         <v>260393.21</v>
@@ -542,7 +542,7 @@
         <v>77.51000000000001</v>
       </c>
       <c r="D4" t="n">
-        <v>0.06</v>
+        <v>3877.05</v>
       </c>
       <c r="E4" t="n">
         <v>59247.72</v>
@@ -570,7 +570,7 @@
         <v>144.72</v>
       </c>
       <c r="D5" t="n">
-        <v>0.19</v>
+        <v>7233.4</v>
       </c>
       <c r="E5" t="n">
         <v>109746.94</v>
@@ -598,7 +598,7 @@
         <v>300.84</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>15055.63</v>
       </c>
       <c r="E6" t="n">
         <v>225448.79</v>
@@ -626,7 +626,7 @@
         <v>382.26</v>
       </c>
       <c r="D7" t="n">
-        <v>0.52</v>
+        <v>19120.08</v>
       </c>
       <c r="E7" t="n">
         <v>287465.6</v>
@@ -654,7 +654,7 @@
         <v>295.1</v>
       </c>
       <c r="D8" t="n">
-        <v>0.42</v>
+        <v>14759.22</v>
       </c>
       <c r="E8" t="n">
         <v>221993.42</v>
@@ -682,7 +682,7 @@
         <v>148.23</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>7412.77</v>
       </c>
       <c r="E9" t="n">
         <v>111540.28</v>
@@ -710,7 +710,7 @@
         <v>317.01</v>
       </c>
       <c r="D10" t="n">
-        <v>0.43</v>
+        <v>15849.58</v>
       </c>
       <c r="E10" t="n">
         <v>238168.83</v>
@@ -738,7 +738,7 @@
         <v>241.44</v>
       </c>
       <c r="D11" t="n">
-        <v>0.25</v>
+        <v>12087.24</v>
       </c>
       <c r="E11" t="n">
         <v>181362.72</v>
@@ -766,7 +766,7 @@
         <v>316.23</v>
       </c>
       <c r="D12" t="n">
-        <v>0.28</v>
+        <v>15803.09</v>
       </c>
       <c r="E12" t="n">
         <v>237578.99</v>
@@ -794,7 +794,7 @@
         <v>258.99</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>12946.84</v>
       </c>
       <c r="E13" t="n">
         <v>195696.91</v>
@@ -822,7 +822,7 @@
         <v>55.58</v>
       </c>
       <c r="D14" t="n">
-        <v>0.01000000000000001</v>
+        <v>2781.76</v>
       </c>
       <c r="E14" t="n">
         <v>41441.76</v>
@@ -850,7 +850,7 @@
         <v>259.93</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>12998.34</v>
       </c>
       <c r="E15" t="n">
         <v>194916.48</v>
@@ -878,7 +878,7 @@
         <v>419.89</v>
       </c>
       <c r="D16" t="n">
-        <v>0.68</v>
+        <v>20984.57</v>
       </c>
       <c r="E16" t="n">
         <v>313949.84</v>
@@ -906,7 +906,7 @@
         <v>257.54</v>
       </c>
       <c r="D17" t="n">
-        <v>0.44</v>
+        <v>12879.2</v>
       </c>
       <c r="E17" t="n">
         <v>194462.18</v>
@@ -934,7 +934,7 @@
         <v>137.03</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>6852.039999999999</v>
       </c>
       <c r="E18" t="n">
         <v>104629.59</v>
@@ -962,7 +962,7 @@
         <v>461.85</v>
       </c>
       <c r="D19" t="n">
-        <v>0.52</v>
+        <v>23108.32</v>
       </c>
       <c r="E19" t="n">
         <v>350397.26</v>
@@ -990,7 +990,7 @@
         <v>455.14</v>
       </c>
       <c r="D20" t="n">
-        <v>0.37</v>
+        <v>22750.27</v>
       </c>
       <c r="E20" t="n">
         <v>344370.1800000001</v>
@@ -1018,7 +1018,7 @@
         <v>415.55</v>
       </c>
       <c r="D21" t="n">
-        <v>0.54</v>
+        <v>20797.95</v>
       </c>
       <c r="E21" t="n">
         <v>312777.25</v>
@@ -1046,7 +1046,7 @@
         <v>250.33</v>
       </c>
       <c r="D22" t="n">
-        <v>0.33</v>
+        <v>12529.67</v>
       </c>
       <c r="E22" t="n">
         <v>188745.84</v>
@@ -1074,7 +1074,7 @@
         <v>197.78</v>
       </c>
       <c r="D23" t="n">
-        <v>0.27</v>
+        <v>9898.040000000001</v>
       </c>
       <c r="E23" t="n">
         <v>150681.27</v>
@@ -1102,7 +1102,7 @@
         <v>591.86</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>29601</v>
       </c>
       <c r="E24" t="n">
         <v>445455.16</v>

</xml_diff>